<commit_message>
adding last models that must be done
also added a lot to asset spreadsheet
</commit_message>
<xml_diff>
--- a/Documents/asset list for deer forest.xlsx
+++ b/Documents/asset list for deer forest.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\deers forest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rediu\Documents\AIE\RepoFolder\DeerForestrepo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71CEA44C-3783-4B6C-B9F5-FF3F0C64B146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C55A1-2769-40D6-B6AF-D20D5320B0D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D00E0E2-157F-465B-873F-A0056DDA9424}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1D00E0E2-157F-465B-873F-A0056DDA9424}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -58,6 +49,150 @@
   </si>
   <si>
     <t>file name</t>
+  </si>
+  <si>
+    <t>Deer Statue</t>
+  </si>
+  <si>
+    <t>mushroom orb</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>shrub</t>
+  </si>
+  <si>
+    <t>grass blade</t>
+  </si>
+  <si>
+    <t>waterfall</t>
+  </si>
+  <si>
+    <t>waterfall bay</t>
+  </si>
+  <si>
+    <t>waterfall stand</t>
+  </si>
+  <si>
+    <t>large tree</t>
+  </si>
+  <si>
+    <t>small tree</t>
+  </si>
+  <si>
+    <t>stone</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>pebble</t>
+  </si>
+  <si>
+    <t>pick-ups</t>
+  </si>
+  <si>
+    <t>feature asset</t>
+  </si>
+  <si>
+    <t>border of map</t>
+  </si>
+  <si>
+    <t>decoration</t>
+  </si>
+  <si>
+    <t>puzzle piece</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>pathway</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decoration </t>
+  </si>
+  <si>
+    <t>deerstatueactualfulltexture</t>
+  </si>
+  <si>
+    <t>orbshroomactual</t>
+  </si>
+  <si>
+    <t>grassblade</t>
+  </si>
+  <si>
+    <t>waterfallbay</t>
+  </si>
+  <si>
+    <t>waterfallstand</t>
+  </si>
+  <si>
+    <t>largetree</t>
+  </si>
+  <si>
+    <t>shrub1</t>
+  </si>
+  <si>
+    <t>smalltreesizetest</t>
+  </si>
+  <si>
+    <t>3x3x3</t>
+  </si>
+  <si>
+    <t>2x2x2</t>
+  </si>
+  <si>
+    <t>1x1x1</t>
+  </si>
+  <si>
+    <t>mapwallsizetest</t>
+  </si>
+  <si>
+    <t>7x13x8</t>
+  </si>
+  <si>
+    <t>0.3x2</t>
+  </si>
+  <si>
+    <t>1x1x1 (multiple upscales)</t>
+  </si>
+  <si>
+    <t>40x60x38</t>
+  </si>
+  <si>
+    <t>4x25x3.5</t>
+  </si>
+  <si>
+    <t>8.5x3.5x14</t>
+  </si>
+  <si>
+    <t>69x7x69</t>
+  </si>
+  <si>
+    <t>70x30x70</t>
+  </si>
+  <si>
+    <t>stump</t>
+  </si>
+  <si>
+    <t>0.5x7</t>
+  </si>
+  <si>
+    <t>0.5x2</t>
+  </si>
+  <si>
+    <t>waterfallwater</t>
+  </si>
+  <si>
+    <t>11.5x11.5x11.5</t>
   </si>
 </sst>
 </file>
@@ -409,23 +544,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E42BCF-39F3-442B-8710-A8D0F674E1DF}">
-  <dimension ref="B2:I2"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -449,6 +586,232 @@
       </c>
       <c r="I2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -457,6 +820,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D386F57F7DCDE4B89632BB855604217" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3f61da04c3c1bed784fd3ad1e98edd1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="20e15830-a185-4db3-af6f-3cdc4ceb4ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68d6c8ea9b2dea1df420bceda759dc5a" ns3:_="">
     <xsd:import namespace="20e15830-a185-4db3-af6f-3cdc4ceb4ee7"/>
@@ -588,22 +966,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8EC6D2C-F6ED-4035-A59F-3DC803559E1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="20e15830-a185-4db3-af6f-3cdc4ceb4ee7"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A80D5A7-0533-4A30-AF90-171231E57542}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3823C695-E823-4F08-A5CD-1455356ADB86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -619,28 +1006,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A80D5A7-0533-4A30-AF90-171231E57542}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8EC6D2C-F6ED-4035-A59F-3DC803559E1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="20e15830-a185-4db3-af6f-3cdc4ceb4ee7"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
save scare added path and wall
texture all.
</commit_message>
<xml_diff>
--- a/Documents/asset list for deer forest.xlsx
+++ b/Documents/asset list for deer forest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rediu\Documents\AIE\RepoFolder\DeerForestrepo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C55A1-2769-40D6-B6AF-D20D5320B0D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B98547E-DA98-4FC7-8B3B-D3563C16FC9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{1D00E0E2-157F-465B-873F-A0056DDA9424}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,21 +820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D386F57F7DCDE4B89632BB855604217" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3f61da04c3c1bed784fd3ad1e98edd1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="20e15830-a185-4db3-af6f-3cdc4ceb4ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68d6c8ea9b2dea1df420bceda759dc5a" ns3:_="">
     <xsd:import namespace="20e15830-a185-4db3-af6f-3cdc4ceb4ee7"/>
@@ -966,31 +951,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8EC6D2C-F6ED-4035-A59F-3DC803559E1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="20e15830-a185-4db3-af6f-3cdc4ceb4ee7"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A80D5A7-0533-4A30-AF90-171231E57542}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3823C695-E823-4F08-A5CD-1455356ADB86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1006,4 +982,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A80D5A7-0533-4A30-AF90-171231E57542}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8EC6D2C-F6ED-4035-A59F-3DC803559E1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="20e15830-a185-4db3-af6f-3cdc4ceb4ee7"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>